<commit_message>
add new Rachel neut data set 2 & configure `yaml`
</commit_message>
<xml_diff>
--- a/data/neut_assays/plate_reader_data/557v2_NeutralizationAssay.xlsx
+++ b/data/neut_assays/plate_reader_data/557v2_NeutralizationAssay.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="34180" yWindow="460" windowWidth="28340" windowHeight="17360" activeTab="2"/>
+    <workbookView xWindow="4280" yWindow="460" windowWidth="28340" windowHeight="16460" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="WT" sheetId="2" r:id="rId1"/>
     <sheet name="F159G" sheetId="1" r:id="rId2"/>
     <sheet name="F159F" sheetId="3" r:id="rId3"/>
+    <sheet name="WT2" sheetId="4" r:id="rId4"/>
+    <sheet name="R220D" sheetId="5" r:id="rId5"/>
+    <sheet name="K189D" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -295,8 +298,275 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="70">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -470,6 +740,42 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>9:32:38 AM</t>
+  </si>
+  <si>
+    <t>FHCRC\reguia</t>
+  </si>
+  <si>
+    <t>5/24/2019 9:33:35 AM</t>
+  </si>
+  <si>
+    <t>Temperature: 24.1 °C</t>
+  </si>
+  <si>
+    <t>5/24/2019 9:34:31 AM</t>
+  </si>
+  <si>
+    <t>9:30:24 AM</t>
+  </si>
+  <si>
+    <t>5/24/2019 9:31:21 AM</t>
+  </si>
+  <si>
+    <t>Temperature: 23.8 °C</t>
+  </si>
+  <si>
+    <t>5/24/2019 9:32:17 AM</t>
+  </si>
+  <si>
+    <t>9:27:59 AM</t>
+  </si>
+  <si>
+    <t>5/24/2019 9:29:05 AM</t>
+  </si>
+  <si>
+    <t>5/24/2019 9:30:00 AM</t>
   </si>
 </sst>
 </file>
@@ -1984,7 +2290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -2509,4 +2815,1813 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43609</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>109</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <v>14038</v>
+      </c>
+      <c r="C32">
+        <v>14676</v>
+      </c>
+      <c r="D32">
+        <v>15141</v>
+      </c>
+      <c r="E32">
+        <v>15640</v>
+      </c>
+      <c r="F32">
+        <v>15757</v>
+      </c>
+      <c r="G32">
+        <v>15536</v>
+      </c>
+      <c r="H32">
+        <v>15996</v>
+      </c>
+      <c r="I32">
+        <v>15778</v>
+      </c>
+      <c r="J32">
+        <v>15441</v>
+      </c>
+      <c r="K32">
+        <v>15203</v>
+      </c>
+      <c r="L32">
+        <v>14700</v>
+      </c>
+      <c r="M32">
+        <v>14107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>21533</v>
+      </c>
+      <c r="C33">
+        <v>21196</v>
+      </c>
+      <c r="D33">
+        <v>22213</v>
+      </c>
+      <c r="E33">
+        <v>22299</v>
+      </c>
+      <c r="F33">
+        <v>22575</v>
+      </c>
+      <c r="G33">
+        <v>22714</v>
+      </c>
+      <c r="H33">
+        <v>22475</v>
+      </c>
+      <c r="I33">
+        <v>22645</v>
+      </c>
+      <c r="J33">
+        <v>22333</v>
+      </c>
+      <c r="K33">
+        <v>21986</v>
+      </c>
+      <c r="L33">
+        <v>21697</v>
+      </c>
+      <c r="M33">
+        <v>21507</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>34683</v>
+      </c>
+      <c r="C34">
+        <v>36917</v>
+      </c>
+      <c r="D34">
+        <v>40816</v>
+      </c>
+      <c r="E34">
+        <v>40817</v>
+      </c>
+      <c r="F34">
+        <v>42261</v>
+      </c>
+      <c r="G34">
+        <v>42085</v>
+      </c>
+      <c r="H34">
+        <v>43295</v>
+      </c>
+      <c r="I34">
+        <v>42283</v>
+      </c>
+      <c r="J34">
+        <v>41813</v>
+      </c>
+      <c r="K34">
+        <v>39249</v>
+      </c>
+      <c r="L34">
+        <v>37434</v>
+      </c>
+      <c r="M34">
+        <v>36223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>32669</v>
+      </c>
+      <c r="C35">
+        <v>36805</v>
+      </c>
+      <c r="D35">
+        <v>37214</v>
+      </c>
+      <c r="E35">
+        <v>37575</v>
+      </c>
+      <c r="F35">
+        <v>34947</v>
+      </c>
+      <c r="G35">
+        <v>30327</v>
+      </c>
+      <c r="H35">
+        <v>25693</v>
+      </c>
+      <c r="I35">
+        <v>22509</v>
+      </c>
+      <c r="J35">
+        <v>21392</v>
+      </c>
+      <c r="K35">
+        <v>20994</v>
+      </c>
+      <c r="L35">
+        <v>21306</v>
+      </c>
+      <c r="M35">
+        <v>21620</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>31364</v>
+      </c>
+      <c r="C36">
+        <v>35562</v>
+      </c>
+      <c r="D36">
+        <v>37403</v>
+      </c>
+      <c r="E36">
+        <v>36040</v>
+      </c>
+      <c r="F36">
+        <v>34146</v>
+      </c>
+      <c r="G36">
+        <v>30027</v>
+      </c>
+      <c r="H36">
+        <v>25890</v>
+      </c>
+      <c r="I36">
+        <v>22606</v>
+      </c>
+      <c r="J36">
+        <v>21224</v>
+      </c>
+      <c r="K36">
+        <v>20856</v>
+      </c>
+      <c r="L36">
+        <v>20748</v>
+      </c>
+      <c r="M36">
+        <v>21582</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>33758</v>
+      </c>
+      <c r="C37">
+        <v>35944</v>
+      </c>
+      <c r="D37">
+        <v>37368</v>
+      </c>
+      <c r="E37">
+        <v>37200</v>
+      </c>
+      <c r="F37">
+        <v>33643</v>
+      </c>
+      <c r="G37">
+        <v>29445</v>
+      </c>
+      <c r="H37">
+        <v>24410</v>
+      </c>
+      <c r="I37">
+        <v>21664</v>
+      </c>
+      <c r="J37">
+        <v>20776</v>
+      </c>
+      <c r="K37">
+        <v>20671</v>
+      </c>
+      <c r="L37">
+        <v>20825</v>
+      </c>
+      <c r="M37">
+        <v>21526</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>33003</v>
+      </c>
+      <c r="C38">
+        <v>35556</v>
+      </c>
+      <c r="D38">
+        <v>39238</v>
+      </c>
+      <c r="E38">
+        <v>36587</v>
+      </c>
+      <c r="F38">
+        <v>38478</v>
+      </c>
+      <c r="G38">
+        <v>40124</v>
+      </c>
+      <c r="H38">
+        <v>36230</v>
+      </c>
+      <c r="I38">
+        <v>38317</v>
+      </c>
+      <c r="J38">
+        <v>39763</v>
+      </c>
+      <c r="K38">
+        <v>35701</v>
+      </c>
+      <c r="L38">
+        <v>35650</v>
+      </c>
+      <c r="M38">
+        <v>33605</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39">
+        <v>13035</v>
+      </c>
+      <c r="C39">
+        <v>13234</v>
+      </c>
+      <c r="D39">
+        <v>13736</v>
+      </c>
+      <c r="E39">
+        <v>14093</v>
+      </c>
+      <c r="F39">
+        <v>14695</v>
+      </c>
+      <c r="G39">
+        <v>14085</v>
+      </c>
+      <c r="H39">
+        <v>14530</v>
+      </c>
+      <c r="I39">
+        <v>14501</v>
+      </c>
+      <c r="J39">
+        <v>13955</v>
+      </c>
+      <c r="K39">
+        <v>13781</v>
+      </c>
+      <c r="L39">
+        <v>13544</v>
+      </c>
+      <c r="M39">
+        <v>12948</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43609</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>109</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <v>13829</v>
+      </c>
+      <c r="C32">
+        <v>14126</v>
+      </c>
+      <c r="D32">
+        <v>15164</v>
+      </c>
+      <c r="E32">
+        <v>15337</v>
+      </c>
+      <c r="F32">
+        <v>15575</v>
+      </c>
+      <c r="G32">
+        <v>15646</v>
+      </c>
+      <c r="H32">
+        <v>15595</v>
+      </c>
+      <c r="I32">
+        <v>14993</v>
+      </c>
+      <c r="J32">
+        <v>15536</v>
+      </c>
+      <c r="K32">
+        <v>14656</v>
+      </c>
+      <c r="L32">
+        <v>14353</v>
+      </c>
+      <c r="M32">
+        <v>13744</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>20352</v>
+      </c>
+      <c r="C33">
+        <v>20355</v>
+      </c>
+      <c r="D33">
+        <v>20666</v>
+      </c>
+      <c r="E33">
+        <v>21084</v>
+      </c>
+      <c r="F33">
+        <v>21162</v>
+      </c>
+      <c r="G33">
+        <v>21536</v>
+      </c>
+      <c r="H33">
+        <v>21016</v>
+      </c>
+      <c r="I33">
+        <v>21232</v>
+      </c>
+      <c r="J33">
+        <v>20988</v>
+      </c>
+      <c r="K33">
+        <v>20750</v>
+      </c>
+      <c r="L33">
+        <v>20009</v>
+      </c>
+      <c r="M33">
+        <v>19974</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>36998</v>
+      </c>
+      <c r="C34">
+        <v>38744</v>
+      </c>
+      <c r="D34">
+        <v>35909</v>
+      </c>
+      <c r="E34">
+        <v>35762</v>
+      </c>
+      <c r="F34">
+        <v>35017</v>
+      </c>
+      <c r="G34">
+        <v>34082</v>
+      </c>
+      <c r="H34">
+        <v>34457</v>
+      </c>
+      <c r="I34">
+        <v>38269</v>
+      </c>
+      <c r="J34">
+        <v>40153</v>
+      </c>
+      <c r="K34">
+        <v>35524</v>
+      </c>
+      <c r="L34">
+        <v>39622</v>
+      </c>
+      <c r="M34">
+        <v>36233</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>35330</v>
+      </c>
+      <c r="C35">
+        <v>37708</v>
+      </c>
+      <c r="D35">
+        <v>35223</v>
+      </c>
+      <c r="E35">
+        <v>39144</v>
+      </c>
+      <c r="F35">
+        <v>34326</v>
+      </c>
+      <c r="G35">
+        <v>31196</v>
+      </c>
+      <c r="H35">
+        <v>28657</v>
+      </c>
+      <c r="I35">
+        <v>25701</v>
+      </c>
+      <c r="J35">
+        <v>20899</v>
+      </c>
+      <c r="K35">
+        <v>19935</v>
+      </c>
+      <c r="L35">
+        <v>19868</v>
+      </c>
+      <c r="M35">
+        <v>20037</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>35472</v>
+      </c>
+      <c r="C36">
+        <v>37367</v>
+      </c>
+      <c r="D36">
+        <v>36636</v>
+      </c>
+      <c r="E36">
+        <v>35563</v>
+      </c>
+      <c r="F36">
+        <v>33489</v>
+      </c>
+      <c r="G36">
+        <v>31151</v>
+      </c>
+      <c r="H36">
+        <v>29365</v>
+      </c>
+      <c r="I36">
+        <v>25234</v>
+      </c>
+      <c r="J36">
+        <v>21055</v>
+      </c>
+      <c r="K36">
+        <v>20041</v>
+      </c>
+      <c r="L36">
+        <v>19633</v>
+      </c>
+      <c r="M36">
+        <v>20545</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>35564</v>
+      </c>
+      <c r="C37">
+        <v>34975</v>
+      </c>
+      <c r="D37">
+        <v>32736</v>
+      </c>
+      <c r="E37">
+        <v>33484</v>
+      </c>
+      <c r="F37">
+        <v>32808</v>
+      </c>
+      <c r="G37">
+        <v>32775</v>
+      </c>
+      <c r="H37">
+        <v>29979</v>
+      </c>
+      <c r="I37">
+        <v>23842</v>
+      </c>
+      <c r="J37">
+        <v>20308</v>
+      </c>
+      <c r="K37">
+        <v>19471</v>
+      </c>
+      <c r="L37">
+        <v>19585</v>
+      </c>
+      <c r="M37">
+        <v>20066</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>34678</v>
+      </c>
+      <c r="C38">
+        <v>36176</v>
+      </c>
+      <c r="D38">
+        <v>33911</v>
+      </c>
+      <c r="E38">
+        <v>35304</v>
+      </c>
+      <c r="F38">
+        <v>34098</v>
+      </c>
+      <c r="G38">
+        <v>34381</v>
+      </c>
+      <c r="H38">
+        <v>35324</v>
+      </c>
+      <c r="I38">
+        <v>34932</v>
+      </c>
+      <c r="J38">
+        <v>35916</v>
+      </c>
+      <c r="K38">
+        <v>34305</v>
+      </c>
+      <c r="L38">
+        <v>34766</v>
+      </c>
+      <c r="M38">
+        <v>36505</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39">
+        <v>13482</v>
+      </c>
+      <c r="C39">
+        <v>13392</v>
+      </c>
+      <c r="D39">
+        <v>13569</v>
+      </c>
+      <c r="E39">
+        <v>13968</v>
+      </c>
+      <c r="F39">
+        <v>14260</v>
+      </c>
+      <c r="G39">
+        <v>14462</v>
+      </c>
+      <c r="H39">
+        <v>14332</v>
+      </c>
+      <c r="I39">
+        <v>14336</v>
+      </c>
+      <c r="J39">
+        <v>13987</v>
+      </c>
+      <c r="K39">
+        <v>13627</v>
+      </c>
+      <c r="L39">
+        <v>13037</v>
+      </c>
+      <c r="M39">
+        <v>12577</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43609</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>101</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <v>7521</v>
+      </c>
+      <c r="C32">
+        <v>7881</v>
+      </c>
+      <c r="D32">
+        <v>7914</v>
+      </c>
+      <c r="E32">
+        <v>8062</v>
+      </c>
+      <c r="F32">
+        <v>8480</v>
+      </c>
+      <c r="G32">
+        <v>8462</v>
+      </c>
+      <c r="H32">
+        <v>8289</v>
+      </c>
+      <c r="I32">
+        <v>8161</v>
+      </c>
+      <c r="J32">
+        <v>8195</v>
+      </c>
+      <c r="K32">
+        <v>8015</v>
+      </c>
+      <c r="L32">
+        <v>7866</v>
+      </c>
+      <c r="M32">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>9872</v>
+      </c>
+      <c r="C33">
+        <v>10038</v>
+      </c>
+      <c r="D33">
+        <v>10290</v>
+      </c>
+      <c r="E33">
+        <v>10239</v>
+      </c>
+      <c r="F33">
+        <v>10444</v>
+      </c>
+      <c r="G33">
+        <v>10602</v>
+      </c>
+      <c r="H33">
+        <v>10415</v>
+      </c>
+      <c r="I33">
+        <v>10259</v>
+      </c>
+      <c r="J33">
+        <v>10310</v>
+      </c>
+      <c r="K33">
+        <v>10131</v>
+      </c>
+      <c r="L33">
+        <v>9988</v>
+      </c>
+      <c r="M33">
+        <v>9773</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>27657</v>
+      </c>
+      <c r="C34">
+        <v>32079</v>
+      </c>
+      <c r="D34">
+        <v>34689</v>
+      </c>
+      <c r="E34">
+        <v>34608</v>
+      </c>
+      <c r="F34">
+        <v>35174</v>
+      </c>
+      <c r="G34">
+        <v>36574</v>
+      </c>
+      <c r="H34">
+        <v>35442</v>
+      </c>
+      <c r="I34">
+        <v>36274</v>
+      </c>
+      <c r="J34">
+        <v>36139</v>
+      </c>
+      <c r="K34">
+        <v>34153</v>
+      </c>
+      <c r="L34">
+        <v>33683</v>
+      </c>
+      <c r="M34">
+        <v>31033</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>28279</v>
+      </c>
+      <c r="C35">
+        <v>31505</v>
+      </c>
+      <c r="D35">
+        <v>33110</v>
+      </c>
+      <c r="E35">
+        <v>31533</v>
+      </c>
+      <c r="F35">
+        <v>29886</v>
+      </c>
+      <c r="G35">
+        <v>28213</v>
+      </c>
+      <c r="H35">
+        <v>22722</v>
+      </c>
+      <c r="I35">
+        <v>16595</v>
+      </c>
+      <c r="J35">
+        <v>12397</v>
+      </c>
+      <c r="K35">
+        <v>10098</v>
+      </c>
+      <c r="L35">
+        <v>9503</v>
+      </c>
+      <c r="M35">
+        <v>9848</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>29823</v>
+      </c>
+      <c r="C36">
+        <v>29160</v>
+      </c>
+      <c r="D36">
+        <v>31901</v>
+      </c>
+      <c r="E36">
+        <v>32778</v>
+      </c>
+      <c r="F36">
+        <v>30292</v>
+      </c>
+      <c r="G36">
+        <v>27019</v>
+      </c>
+      <c r="H36">
+        <v>20960</v>
+      </c>
+      <c r="I36">
+        <v>16237</v>
+      </c>
+      <c r="J36">
+        <v>12745</v>
+      </c>
+      <c r="K36">
+        <v>9994</v>
+      </c>
+      <c r="L36">
+        <v>9577</v>
+      </c>
+      <c r="M36">
+        <v>9607</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>29727</v>
+      </c>
+      <c r="C37">
+        <v>28292</v>
+      </c>
+      <c r="D37">
+        <v>28466</v>
+      </c>
+      <c r="E37">
+        <v>30317</v>
+      </c>
+      <c r="F37">
+        <v>29452</v>
+      </c>
+      <c r="G37">
+        <v>26333</v>
+      </c>
+      <c r="H37">
+        <v>21797</v>
+      </c>
+      <c r="I37">
+        <v>16486</v>
+      </c>
+      <c r="J37">
+        <v>12202</v>
+      </c>
+      <c r="K37">
+        <v>9938</v>
+      </c>
+      <c r="L37">
+        <v>9633</v>
+      </c>
+      <c r="M37">
+        <v>9618</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>26386</v>
+      </c>
+      <c r="C38">
+        <v>26886</v>
+      </c>
+      <c r="D38">
+        <v>30984</v>
+      </c>
+      <c r="E38">
+        <v>30315</v>
+      </c>
+      <c r="F38">
+        <v>31601</v>
+      </c>
+      <c r="G38">
+        <v>32697</v>
+      </c>
+      <c r="H38">
+        <v>31742</v>
+      </c>
+      <c r="I38">
+        <v>33336</v>
+      </c>
+      <c r="J38">
+        <v>35088</v>
+      </c>
+      <c r="K38">
+        <v>31291</v>
+      </c>
+      <c r="L38">
+        <v>30089</v>
+      </c>
+      <c r="M38">
+        <v>28305</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39">
+        <v>7044</v>
+      </c>
+      <c r="C39">
+        <v>7508</v>
+      </c>
+      <c r="D39">
+        <v>7308</v>
+      </c>
+      <c r="E39">
+        <v>7435</v>
+      </c>
+      <c r="F39">
+        <v>7683</v>
+      </c>
+      <c r="G39">
+        <v>7717</v>
+      </c>
+      <c r="H39">
+        <v>7726</v>
+      </c>
+      <c r="I39">
+        <v>7584</v>
+      </c>
+      <c r="J39">
+        <v>7392</v>
+      </c>
+      <c r="K39">
+        <v>7306</v>
+      </c>
+      <c r="L39">
+        <v>7012</v>
+      </c>
+      <c r="M39">
+        <v>6811</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
analyze new neut data, set 2
</commit_message>
<xml_diff>
--- a/data/neut_assays/plate_reader_data/557v2_NeutralizationAssay.xlsx
+++ b/data/neut_assays/plate_reader_data/557v2_NeutralizationAssay.xlsx
@@ -1,28 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhyemlee/Google Drive/Bloom_Lab/Perth2009_MAP/NeutralizationAssays/mutvalidation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="34180" yWindow="460" windowWidth="28340" windowHeight="17360" activeTab="2"/>
+    <workbookView xWindow="6800" yWindow="1260" windowWidth="28340" windowHeight="16460" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="WT" sheetId="2" r:id="rId1"/>
     <sheet name="F159G" sheetId="1" r:id="rId2"/>
     <sheet name="F159F" sheetId="3" r:id="rId3"/>
+    <sheet name="WT2" sheetId="4" r:id="rId4"/>
+    <sheet name="R220D" sheetId="5" r:id="rId5"/>
+    <sheet name="K189D" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -295,8 +293,275 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="69">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -470,6 +735,39 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>FHCRC\reguia</t>
+  </si>
+  <si>
+    <t>Temperature: 23.8 °C</t>
+  </si>
+  <si>
+    <t>9:35:38 AM</t>
+  </si>
+  <si>
+    <t>5/28/2019 9:36:42 AM</t>
+  </si>
+  <si>
+    <t>5/28/2019 9:37:37 AM</t>
+  </si>
+  <si>
+    <t>9:33:21 AM</t>
+  </si>
+  <si>
+    <t>5/28/2019 9:34:24 AM</t>
+  </si>
+  <si>
+    <t>5/28/2019 9:35:20 AM</t>
+  </si>
+  <si>
+    <t>9:31:00 AM</t>
+  </si>
+  <si>
+    <t>5/28/2019 9:32:08 AM</t>
+  </si>
+  <si>
+    <t>5/28/2019 9:33:04 AM</t>
   </si>
 </sst>
 </file>
@@ -676,7 +974,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -711,7 +1009,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -926,9 +1224,9 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -936,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -944,7 +1242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -952,7 +1250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -960,7 +1258,7 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -968,7 +1266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -976,7 +1274,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -984,7 +1282,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -992,17 +1290,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1010,12 +1308,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1026,7 +1324,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1037,7 +1335,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1048,7 +1346,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1059,7 +1357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1070,7 +1368,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1081,7 +1379,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1092,7 +1390,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1103,7 +1401,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1114,7 +1412,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1125,7 +1423,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1133,12 +1431,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1179,12 +1477,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -1225,7 +1523,7 @@
         <v>9302</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -1266,7 +1564,7 @@
         <v>27616</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -1307,7 +1605,7 @@
         <v>9113</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -1348,7 +1646,7 @@
         <v>9279</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -1389,7 +1687,7 @@
         <v>9285</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -1430,12 +1728,12 @@
         <v>20872</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1446,6 +1744,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1457,9 +1760,9 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1467,7 +1770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1475,7 +1778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1483,7 +1786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1491,7 +1794,7 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1499,7 +1802,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1507,7 +1810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1515,7 +1818,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1523,17 +1826,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1541,12 +1844,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1557,7 +1860,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1568,7 +1871,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1579,7 +1882,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1590,7 +1893,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1601,7 +1904,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1612,7 +1915,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1623,7 +1926,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1634,7 +1937,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1645,7 +1948,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1656,7 +1959,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1664,12 +1967,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1710,12 +2013,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -1756,7 +2059,7 @@
         <v>5659</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -1797,7 +2100,7 @@
         <v>25363</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -1838,7 +2141,7 @@
         <v>24495</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -1879,7 +2182,7 @@
         <v>23629</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -1920,7 +2223,7 @@
         <v>22867</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -1961,12 +2264,12 @@
         <v>23260</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1977,6 +2280,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1984,13 +2292,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1998,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2006,7 +2314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2014,7 +2322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2022,7 +2330,7 @@
         <v>43581</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2030,7 +2338,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2038,7 +2346,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2046,7 +2354,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2054,17 +2362,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2072,12 +2380,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2088,7 +2396,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2099,7 +2407,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2110,7 +2418,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2121,7 +2429,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2132,7 +2440,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2143,7 +2451,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2154,7 +2462,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2165,7 +2473,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2176,7 +2484,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2187,7 +2495,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2195,12 +2503,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -2241,12 +2549,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -2287,7 +2595,7 @@
         <v>10181</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -2328,7 +2636,7 @@
         <v>32031</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -2369,7 +2677,7 @@
         <v>9978</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -2410,7 +2718,7 @@
         <v>10076</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -2451,7 +2759,7 @@
         <v>10069</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -2492,12 +2800,12 @@
         <v>28597</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2508,5 +2816,1834 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B33" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>94</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <v>4523</v>
+      </c>
+      <c r="C32">
+        <v>4658</v>
+      </c>
+      <c r="D32">
+        <v>4992</v>
+      </c>
+      <c r="E32">
+        <v>5116</v>
+      </c>
+      <c r="F32">
+        <v>5187</v>
+      </c>
+      <c r="G32">
+        <v>5150</v>
+      </c>
+      <c r="H32">
+        <v>5228</v>
+      </c>
+      <c r="I32">
+        <v>5039</v>
+      </c>
+      <c r="J32">
+        <v>5164</v>
+      </c>
+      <c r="K32">
+        <v>4915</v>
+      </c>
+      <c r="L32">
+        <v>4851</v>
+      </c>
+      <c r="M32">
+        <v>4702</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>8434</v>
+      </c>
+      <c r="C33">
+        <v>8517</v>
+      </c>
+      <c r="D33">
+        <v>8626</v>
+      </c>
+      <c r="E33">
+        <v>8767</v>
+      </c>
+      <c r="F33">
+        <v>8749</v>
+      </c>
+      <c r="G33">
+        <v>8919</v>
+      </c>
+      <c r="H33">
+        <v>8744</v>
+      </c>
+      <c r="I33">
+        <v>8839</v>
+      </c>
+      <c r="J33">
+        <v>8726</v>
+      </c>
+      <c r="K33">
+        <v>8833</v>
+      </c>
+      <c r="L33">
+        <v>8567</v>
+      </c>
+      <c r="M33">
+        <v>8612</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>24619</v>
+      </c>
+      <c r="C34">
+        <v>28396</v>
+      </c>
+      <c r="D34">
+        <v>29749</v>
+      </c>
+      <c r="E34">
+        <v>32634</v>
+      </c>
+      <c r="F34">
+        <v>32708</v>
+      </c>
+      <c r="G34">
+        <v>34638</v>
+      </c>
+      <c r="H34">
+        <v>33614</v>
+      </c>
+      <c r="I34">
+        <v>34086</v>
+      </c>
+      <c r="J34">
+        <v>33848</v>
+      </c>
+      <c r="K34">
+        <v>34071</v>
+      </c>
+      <c r="L34">
+        <v>31776</v>
+      </c>
+      <c r="M34">
+        <v>29924</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>24196</v>
+      </c>
+      <c r="C35">
+        <v>29344</v>
+      </c>
+      <c r="D35">
+        <v>28700</v>
+      </c>
+      <c r="E35">
+        <v>30435</v>
+      </c>
+      <c r="F35">
+        <v>34276</v>
+      </c>
+      <c r="G35">
+        <v>33569</v>
+      </c>
+      <c r="H35">
+        <v>31471</v>
+      </c>
+      <c r="I35">
+        <v>22310</v>
+      </c>
+      <c r="J35">
+        <v>9688</v>
+      </c>
+      <c r="K35">
+        <v>8143</v>
+      </c>
+      <c r="L35">
+        <v>8182</v>
+      </c>
+      <c r="M35">
+        <v>8207</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>24858</v>
+      </c>
+      <c r="C36">
+        <v>27036</v>
+      </c>
+      <c r="D36">
+        <v>28177</v>
+      </c>
+      <c r="E36">
+        <v>30953</v>
+      </c>
+      <c r="F36">
+        <v>32688</v>
+      </c>
+      <c r="G36">
+        <v>30941</v>
+      </c>
+      <c r="H36">
+        <v>29875</v>
+      </c>
+      <c r="I36">
+        <v>20271</v>
+      </c>
+      <c r="J36">
+        <v>9295</v>
+      </c>
+      <c r="K36">
+        <v>8102</v>
+      </c>
+      <c r="L36">
+        <v>8142</v>
+      </c>
+      <c r="M36">
+        <v>8408</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>24319</v>
+      </c>
+      <c r="C37">
+        <v>26190</v>
+      </c>
+      <c r="D37">
+        <v>27152</v>
+      </c>
+      <c r="E37">
+        <v>31252</v>
+      </c>
+      <c r="F37">
+        <v>29699</v>
+      </c>
+      <c r="G37">
+        <v>30617</v>
+      </c>
+      <c r="H37">
+        <v>29342</v>
+      </c>
+      <c r="I37">
+        <v>18578</v>
+      </c>
+      <c r="J37">
+        <v>8983</v>
+      </c>
+      <c r="K37">
+        <v>8003</v>
+      </c>
+      <c r="L37">
+        <v>8084</v>
+      </c>
+      <c r="M37">
+        <v>8317</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>24324</v>
+      </c>
+      <c r="C38">
+        <v>26563</v>
+      </c>
+      <c r="D38">
+        <v>30839</v>
+      </c>
+      <c r="E38">
+        <v>28081</v>
+      </c>
+      <c r="F38">
+        <v>30279</v>
+      </c>
+      <c r="G38">
+        <v>30928</v>
+      </c>
+      <c r="H38">
+        <v>32437</v>
+      </c>
+      <c r="I38">
+        <v>31567</v>
+      </c>
+      <c r="J38">
+        <v>31631</v>
+      </c>
+      <c r="K38">
+        <v>32411</v>
+      </c>
+      <c r="L38">
+        <v>31225</v>
+      </c>
+      <c r="M38">
+        <v>28504</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39">
+        <v>4405</v>
+      </c>
+      <c r="C39">
+        <v>4269</v>
+      </c>
+      <c r="D39">
+        <v>4396</v>
+      </c>
+      <c r="E39">
+        <v>4592</v>
+      </c>
+      <c r="F39">
+        <v>4593</v>
+      </c>
+      <c r="G39">
+        <v>4649</v>
+      </c>
+      <c r="H39">
+        <v>4678</v>
+      </c>
+      <c r="I39">
+        <v>4621</v>
+      </c>
+      <c r="J39">
+        <v>4604</v>
+      </c>
+      <c r="K39">
+        <v>4500</v>
+      </c>
+      <c r="L39">
+        <v>4279</v>
+      </c>
+      <c r="M39">
+        <v>4152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>97</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <v>5799</v>
+      </c>
+      <c r="C32">
+        <v>5829</v>
+      </c>
+      <c r="D32">
+        <v>6076</v>
+      </c>
+      <c r="E32">
+        <v>6200</v>
+      </c>
+      <c r="F32">
+        <v>6369</v>
+      </c>
+      <c r="G32">
+        <v>6385</v>
+      </c>
+      <c r="H32">
+        <v>6387</v>
+      </c>
+      <c r="I32">
+        <v>6366</v>
+      </c>
+      <c r="J32">
+        <v>6173</v>
+      </c>
+      <c r="K32">
+        <v>6004</v>
+      </c>
+      <c r="L32">
+        <v>5838</v>
+      </c>
+      <c r="M32">
+        <v>5656</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>8228</v>
+      </c>
+      <c r="C33">
+        <v>8330</v>
+      </c>
+      <c r="D33">
+        <v>8454</v>
+      </c>
+      <c r="E33">
+        <v>8584</v>
+      </c>
+      <c r="F33">
+        <v>8658</v>
+      </c>
+      <c r="G33">
+        <v>8763</v>
+      </c>
+      <c r="H33">
+        <v>8778</v>
+      </c>
+      <c r="I33">
+        <v>8784</v>
+      </c>
+      <c r="J33">
+        <v>8602</v>
+      </c>
+      <c r="K33">
+        <v>8564</v>
+      </c>
+      <c r="L33">
+        <v>8400</v>
+      </c>
+      <c r="M33">
+        <v>8332</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>25393</v>
+      </c>
+      <c r="C34">
+        <v>28037</v>
+      </c>
+      <c r="D34">
+        <v>30505</v>
+      </c>
+      <c r="E34">
+        <v>30480</v>
+      </c>
+      <c r="F34">
+        <v>30766</v>
+      </c>
+      <c r="G34">
+        <v>33362</v>
+      </c>
+      <c r="H34">
+        <v>33231</v>
+      </c>
+      <c r="I34">
+        <v>32853</v>
+      </c>
+      <c r="J34">
+        <v>31218</v>
+      </c>
+      <c r="K34">
+        <v>31547</v>
+      </c>
+      <c r="L34">
+        <v>29114</v>
+      </c>
+      <c r="M34">
+        <v>28780</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>25141</v>
+      </c>
+      <c r="C35">
+        <v>28646</v>
+      </c>
+      <c r="D35">
+        <v>29062</v>
+      </c>
+      <c r="E35">
+        <v>30379</v>
+      </c>
+      <c r="F35">
+        <v>32266</v>
+      </c>
+      <c r="G35">
+        <v>30915</v>
+      </c>
+      <c r="H35">
+        <v>30485</v>
+      </c>
+      <c r="I35">
+        <v>24163</v>
+      </c>
+      <c r="J35">
+        <v>12609</v>
+      </c>
+      <c r="K35">
+        <v>8511</v>
+      </c>
+      <c r="L35">
+        <v>8023</v>
+      </c>
+      <c r="M35">
+        <v>8165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>24526</v>
+      </c>
+      <c r="C36">
+        <v>27553</v>
+      </c>
+      <c r="D36">
+        <v>29544</v>
+      </c>
+      <c r="E36">
+        <v>29735</v>
+      </c>
+      <c r="F36">
+        <v>32083</v>
+      </c>
+      <c r="G36">
+        <v>29769</v>
+      </c>
+      <c r="H36">
+        <v>31980</v>
+      </c>
+      <c r="I36">
+        <v>22830</v>
+      </c>
+      <c r="J36">
+        <v>11773</v>
+      </c>
+      <c r="K36">
+        <v>8549</v>
+      </c>
+      <c r="L36">
+        <v>8086</v>
+      </c>
+      <c r="M36">
+        <v>8158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>25735</v>
+      </c>
+      <c r="C37">
+        <v>26095</v>
+      </c>
+      <c r="D37">
+        <v>29411</v>
+      </c>
+      <c r="E37">
+        <v>29724</v>
+      </c>
+      <c r="F37">
+        <v>30947</v>
+      </c>
+      <c r="G37">
+        <v>28748</v>
+      </c>
+      <c r="H37">
+        <v>30219</v>
+      </c>
+      <c r="I37">
+        <v>23164</v>
+      </c>
+      <c r="J37">
+        <v>11254</v>
+      </c>
+      <c r="K37">
+        <v>8291</v>
+      </c>
+      <c r="L37">
+        <v>8005</v>
+      </c>
+      <c r="M37">
+        <v>8113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>23941</v>
+      </c>
+      <c r="C38">
+        <v>24576</v>
+      </c>
+      <c r="D38">
+        <v>25979</v>
+      </c>
+      <c r="E38">
+        <v>27993</v>
+      </c>
+      <c r="F38">
+        <v>28960</v>
+      </c>
+      <c r="G38">
+        <v>29383</v>
+      </c>
+      <c r="H38">
+        <v>29516</v>
+      </c>
+      <c r="I38">
+        <v>31512</v>
+      </c>
+      <c r="J38">
+        <v>30266</v>
+      </c>
+      <c r="K38">
+        <v>29005</v>
+      </c>
+      <c r="L38">
+        <v>27845</v>
+      </c>
+      <c r="M38">
+        <v>24121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39">
+        <v>5577</v>
+      </c>
+      <c r="C39">
+        <v>5174</v>
+      </c>
+      <c r="D39">
+        <v>5414</v>
+      </c>
+      <c r="E39">
+        <v>5610</v>
+      </c>
+      <c r="F39">
+        <v>5736</v>
+      </c>
+      <c r="G39">
+        <v>5721</v>
+      </c>
+      <c r="H39">
+        <v>5831</v>
+      </c>
+      <c r="I39">
+        <v>5749</v>
+      </c>
+      <c r="J39">
+        <v>5669</v>
+      </c>
+      <c r="K39">
+        <v>5497</v>
+      </c>
+      <c r="L39">
+        <v>5393</v>
+      </c>
+      <c r="M39">
+        <v>5252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>97</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32">
+        <v>5593</v>
+      </c>
+      <c r="C32">
+        <v>5670</v>
+      </c>
+      <c r="D32">
+        <v>5866</v>
+      </c>
+      <c r="E32">
+        <v>6051</v>
+      </c>
+      <c r="F32">
+        <v>6179</v>
+      </c>
+      <c r="G32">
+        <v>6137</v>
+      </c>
+      <c r="H32">
+        <v>6198</v>
+      </c>
+      <c r="I32">
+        <v>6168</v>
+      </c>
+      <c r="J32">
+        <v>5986</v>
+      </c>
+      <c r="K32">
+        <v>5856</v>
+      </c>
+      <c r="L32">
+        <v>5707</v>
+      </c>
+      <c r="M32">
+        <v>5451</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>7275</v>
+      </c>
+      <c r="C33">
+        <v>7375</v>
+      </c>
+      <c r="D33">
+        <v>7455</v>
+      </c>
+      <c r="E33">
+        <v>7607</v>
+      </c>
+      <c r="F33">
+        <v>7694</v>
+      </c>
+      <c r="G33">
+        <v>7786</v>
+      </c>
+      <c r="H33">
+        <v>7870</v>
+      </c>
+      <c r="I33">
+        <v>7739</v>
+      </c>
+      <c r="J33">
+        <v>7649</v>
+      </c>
+      <c r="K33">
+        <v>7525</v>
+      </c>
+      <c r="L33">
+        <v>7336</v>
+      </c>
+      <c r="M33">
+        <v>7310</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>26512</v>
+      </c>
+      <c r="C34">
+        <v>30453</v>
+      </c>
+      <c r="D34">
+        <v>31475</v>
+      </c>
+      <c r="E34">
+        <v>33420</v>
+      </c>
+      <c r="F34">
+        <v>34326</v>
+      </c>
+      <c r="G34">
+        <v>33281</v>
+      </c>
+      <c r="H34">
+        <v>35527</v>
+      </c>
+      <c r="I34">
+        <v>34435</v>
+      </c>
+      <c r="J34">
+        <v>34337</v>
+      </c>
+      <c r="K34">
+        <v>32853</v>
+      </c>
+      <c r="L34">
+        <v>31300</v>
+      </c>
+      <c r="M34">
+        <v>27915</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>26896</v>
+      </c>
+      <c r="C35">
+        <v>30700</v>
+      </c>
+      <c r="D35">
+        <v>31839</v>
+      </c>
+      <c r="E35">
+        <v>33094</v>
+      </c>
+      <c r="F35">
+        <v>32974</v>
+      </c>
+      <c r="G35">
+        <v>32904</v>
+      </c>
+      <c r="H35">
+        <v>29051</v>
+      </c>
+      <c r="I35">
+        <v>22255</v>
+      </c>
+      <c r="J35">
+        <v>13717</v>
+      </c>
+      <c r="K35">
+        <v>8900</v>
+      </c>
+      <c r="L35">
+        <v>7170</v>
+      </c>
+      <c r="M35">
+        <v>7183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>26425</v>
+      </c>
+      <c r="C36">
+        <v>29703</v>
+      </c>
+      <c r="D36">
+        <v>32186</v>
+      </c>
+      <c r="E36">
+        <v>32103</v>
+      </c>
+      <c r="F36">
+        <v>32510</v>
+      </c>
+      <c r="G36">
+        <v>31555</v>
+      </c>
+      <c r="H36">
+        <v>29447</v>
+      </c>
+      <c r="I36">
+        <v>21594</v>
+      </c>
+      <c r="J36">
+        <v>13103</v>
+      </c>
+      <c r="K36">
+        <v>8360</v>
+      </c>
+      <c r="L36">
+        <v>7176</v>
+      </c>
+      <c r="M36">
+        <v>7165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>25439</v>
+      </c>
+      <c r="C37">
+        <v>28773</v>
+      </c>
+      <c r="D37">
+        <v>30791</v>
+      </c>
+      <c r="E37">
+        <v>31652</v>
+      </c>
+      <c r="F37">
+        <v>30735</v>
+      </c>
+      <c r="G37">
+        <v>30299</v>
+      </c>
+      <c r="H37">
+        <v>29895</v>
+      </c>
+      <c r="I37">
+        <v>21047</v>
+      </c>
+      <c r="J37">
+        <v>13395</v>
+      </c>
+      <c r="K37">
+        <v>8591</v>
+      </c>
+      <c r="L37">
+        <v>7034</v>
+      </c>
+      <c r="M37">
+        <v>7138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>23568</v>
+      </c>
+      <c r="C38">
+        <v>27804</v>
+      </c>
+      <c r="D38">
+        <v>28837</v>
+      </c>
+      <c r="E38">
+        <v>30319</v>
+      </c>
+      <c r="F38">
+        <v>30671</v>
+      </c>
+      <c r="G38">
+        <v>31412</v>
+      </c>
+      <c r="H38">
+        <v>32263</v>
+      </c>
+      <c r="I38">
+        <v>30912</v>
+      </c>
+      <c r="J38">
+        <v>30972</v>
+      </c>
+      <c r="K38">
+        <v>30009</v>
+      </c>
+      <c r="L38">
+        <v>29070</v>
+      </c>
+      <c r="M38">
+        <v>26033</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39">
+        <v>5106</v>
+      </c>
+      <c r="C39">
+        <v>5033</v>
+      </c>
+      <c r="D39">
+        <v>5290</v>
+      </c>
+      <c r="E39">
+        <v>5392</v>
+      </c>
+      <c r="F39">
+        <v>5533</v>
+      </c>
+      <c r="G39">
+        <v>5587</v>
+      </c>
+      <c r="H39">
+        <v>5552</v>
+      </c>
+      <c r="I39">
+        <v>5531</v>
+      </c>
+      <c r="J39">
+        <v>5366</v>
+      </c>
+      <c r="K39">
+        <v>5248</v>
+      </c>
+      <c r="L39">
+        <v>5112</v>
+      </c>
+      <c r="M39">
+        <v>5032</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>